<commit_message>
Updated Git commands list
</commit_message>
<xml_diff>
--- a/DAY04/GitNotes.xlsx
+++ b/DAY04/GitNotes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raji\ChristmasCodingChallenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raji\Christmas_Coding_Challenge_2024\DAY04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F4E69-C144-43F7-A094-26801060BB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5CE94F-33F8-4C61-BEB1-25A508C91924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EDF726C0-36B6-4F5E-ABAC-FD1D0FF1AD54}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="144">
   <si>
     <t>pwd</t>
   </si>
@@ -334,6 +334,138 @@
   </si>
   <si>
     <t>shows list of all customizable settings for system</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>shows all branches in a project</t>
+  </si>
+  <si>
+    <t>git checkout -b &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>create a new branch</t>
+  </si>
+  <si>
+    <t>git diff main &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>check difference between main and branch</t>
+  </si>
+  <si>
+    <t>git checkout &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>switch to a branch</t>
+  </si>
+  <si>
+    <t>git merge &lt;source&gt; &lt;destination&gt;</t>
+  </si>
+  <si>
+    <t>merge branches e.g. git merge branch123 main</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Conflicts</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt; HEAD</t>
+  </si>
+  <si>
+    <t>Marks the start of the section with changes from your current branch (HEAD)</t>
+  </si>
+  <si>
+    <t>=======</t>
+  </si>
+  <si>
+    <t>Divides the conflicting changes.</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt; other-branch</t>
+  </si>
+  <si>
+    <t>Marks the end of the section with changes from the branch being merged (other-branch).</t>
+  </si>
+  <si>
+    <t>git init &lt;folder name&gt;</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>Creates a Git repo for the current folder</t>
+  </si>
+  <si>
+    <t>Create a Git repo for the specified folder/project</t>
+  </si>
+  <si>
+    <t>git clone &lt;repo path&gt;</t>
+  </si>
+  <si>
+    <t>Clones the given repo</t>
+  </si>
+  <si>
+    <t>git clone &lt;repo path&gt; &lt;repo name&gt;</t>
+  </si>
+  <si>
+    <t>Clones the given repo with given name</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>git remote</t>
+  </si>
+  <si>
+    <t>lists name of remotes</t>
+  </si>
+  <si>
+    <t>git remote -v</t>
+  </si>
+  <si>
+    <t>returns remote url</t>
+  </si>
+  <si>
+    <t>git remote add &lt;name&gt; &lt;URL&gt;</t>
+  </si>
+  <si>
+    <t>Renames 'main' to the given name (Git automatically names remote as 'main')</t>
+  </si>
+  <si>
+    <t>git fetch origin main</t>
+  </si>
+  <si>
+    <t>git fetch origin &lt;repo name&gt;</t>
+  </si>
+  <si>
+    <t>fetch from origin remote into local repo's main branch</t>
+  </si>
+  <si>
+    <t>fetch from origin remote into local repo's specific branch</t>
+  </si>
+  <si>
+    <t>git merge origin main</t>
+  </si>
+  <si>
+    <t>sync contents between remote and local main branch</t>
+  </si>
+  <si>
+    <t>pull from remote repo to main local branch</t>
+  </si>
+  <si>
+    <t>git  push &lt;remote&gt; &lt;local branch&gt;</t>
+  </si>
+  <si>
+    <t>git  pull &lt;remote&gt; &lt;local branch&gt;</t>
+  </si>
+  <si>
+    <t>push from local branch to remote repo</t>
   </si>
 </sst>
 </file>
@@ -356,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +499,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -383,9 +521,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -701,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E06AC5-8113-4729-A68E-ABAC51F1A68B}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,7 +1381,204 @@
         <v>82</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>